<commit_message>
Ajout Gestion 8 et init gestion 9
</commit_message>
<xml_diff>
--- a/meeting/GestionHedbo_Semaine8.xlsx
+++ b/meeting/GestionHedbo_Semaine8.xlsx
@@ -182,12 +182,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,6 +203,12 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -343,9 +343,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -355,8 +354,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,24 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -773,21 +773,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -809,12 +809,12 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -846,29 +846,29 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="27" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -881,18 +881,18 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -905,7 +905,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
@@ -916,7 +916,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -925,12 +925,12 @@
       <c r="C14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -940,7 +940,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -949,11 +949,11 @@
       <c r="C16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -966,7 +966,7 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="7" t="s">
         <v>15</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="7" t="s">
         <v>32</v>
       </c>
@@ -988,18 +988,18 @@
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="14"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1012,7 +1012,7 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="7" t="s">
         <v>15</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="7" t="s">
         <v>18</v>
       </c>
@@ -1053,15 +1053,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajout gestino semaine 8 update
</commit_message>
<xml_diff>
--- a/meeting/GestionHedbo_Semaine8.xlsx
+++ b/meeting/GestionHedbo_Semaine8.xlsx
@@ -187,12 +187,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
@@ -209,6 +203,12 @@
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -344,7 +344,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -354,8 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -389,7 +388,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -773,21 +773,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -809,12 +809,12 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -846,7 +846,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="9" t="s">
         <v>20</v>
       </c>
@@ -868,7 +868,7 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -881,18 +881,18 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="17"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -905,7 +905,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
@@ -916,7 +916,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -925,11 +925,11 @@
       <c r="C14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="16" t="s">
         <v>10</v>
       </c>
@@ -949,11 +949,11 @@
       <c r="C16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -966,7 +966,7 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="7" t="s">
         <v>15</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="7" t="s">
         <v>32</v>
       </c>
@@ -988,18 +988,18 @@
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="30"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1012,7 +1012,7 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="7" t="s">
         <v>15</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="7" t="s">
         <v>18</v>
       </c>

</xml_diff>